<commit_message>
Actualizar contenido de las carpetas
</commit_message>
<xml_diff>
--- a/Datos/Compiladodecirugiasfinal.xlsx
+++ b/Datos/Compiladodecirugiasfinal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nataly Rodriguez\OneDrive\Documentos\PruebasAnalisis\pruebasPython\AnalisisPruebaPiloto\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nataly Rodriguez\Documents\AnalisisPruebaPilotoOptiSurge\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A08D8A4-97DE-4CD1-9C40-3FFE559C3714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4A1EAA-1CC8-4C0D-8668-9C9021BC3272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,7 +802,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="U16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V27" sqref="V27"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3612,6 +3612,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1ae9cdc8-cb5f-4b90-a995-a55020e23403" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6b3902c-f109-4919-a292-2351a7767e7b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006474F5E541087541967FF5A23A2764FD" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c312e0f90c0122b5ae53a7f1001d1275">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6b3902c-f109-4919-a292-2351a7767e7b" xmlns:ns3="1ae9cdc8-cb5f-4b90-a995-a55020e23403" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0838d06283d9e264a55896b4845989f6" ns2:_="" ns3:_="">
     <xsd:import namespace="f6b3902c-f109-4919-a292-2351a7767e7b"/>
@@ -3840,27 +3860,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4450FA85-4E6C-465A-94FF-64BAF436FA89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1ae9cdc8-cb5f-4b90-a995-a55020e23403"/>
+    <ds:schemaRef ds:uri="f6b3902c-f109-4919-a292-2351a7767e7b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1ae9cdc8-cb5f-4b90-a995-a55020e23403" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f6b3902c-f109-4919-a292-2351a7767e7b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76B9D92-4038-4301-8978-431923B94AE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BF3BDEE-C95D-4DE1-9099-CD57F90FB88B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3877,29 +3902,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76B9D92-4038-4301-8978-431923B94AE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4450FA85-4E6C-465A-94FF-64BAF436FA89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1ae9cdc8-cb5f-4b90-a995-a55020e23403"/>
-    <ds:schemaRef ds:uri="f6b3902c-f109-4919-a292-2351a7767e7b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>